<commit_message>
Need more mechanism on catalysed reaction
</commit_message>
<xml_diff>
--- a/LaTeX/Experiment/Results/NonCatalyst.xlsx
+++ b/LaTeX/Experiment/Results/NonCatalyst.xlsx
@@ -687,11 +687,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="100481664"/>
-        <c:axId val="100487936"/>
+        <c:axId val="100196352"/>
+        <c:axId val="100198272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="100481664"/>
+        <c:axId val="100196352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -719,7 +719,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100487936"/>
+        <c:crossAx val="100198272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -727,7 +727,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100487936"/>
+        <c:axId val="100198272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -756,7 +756,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100481664"/>
+        <c:crossAx val="100196352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -820,6 +820,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -943,11 +944,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="98825344"/>
-        <c:axId val="98827264"/>
+        <c:axId val="149580032"/>
+        <c:axId val="149586304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="98825344"/>
+        <c:axId val="149580032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -971,6 +972,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -987,7 +989,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98827264"/>
+        <c:crossAx val="149586304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -995,7 +997,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98827264"/>
+        <c:axId val="149586304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1019,6 +1021,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1035,7 +1038,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98825344"/>
+        <c:crossAx val="149580032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1389,11 +1392,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="105522688"/>
-        <c:axId val="105524608"/>
+        <c:axId val="163502720"/>
+        <c:axId val="164631296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="105522688"/>
+        <c:axId val="163502720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1421,7 +1424,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105524608"/>
+        <c:crossAx val="164631296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1429,7 +1432,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105524608"/>
+        <c:axId val="164631296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1458,7 +1461,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105522688"/>
+        <c:crossAx val="163502720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1522,7 +1525,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1655,11 +1657,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="106791680"/>
-        <c:axId val="106793600"/>
+        <c:axId val="164652928"/>
+        <c:axId val="164659200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106791680"/>
+        <c:axId val="164652928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1681,7 +1683,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1698,7 +1699,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="106793600"/>
+        <c:crossAx val="164659200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1706,7 +1707,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106793600"/>
+        <c:axId val="164659200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1730,7 +1731,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1747,7 +1747,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="106791680"/>
+        <c:crossAx val="164652928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1789,7 +1789,15 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Progress Graph for</a:t>
+              <a:t>Rate vs Concentration</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> Graph </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>for</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
@@ -1854,7 +1862,7 @@
                   <c:v>0.185</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.44025700000000001</c:v>
+                  <c:v>0.38431399999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.29223300000000002</c:v>
@@ -1877,11 +1885,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="105622912"/>
-        <c:axId val="105625088"/>
+        <c:axId val="166273792"/>
+        <c:axId val="166275712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="105622912"/>
+        <c:axId val="166273792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1933,7 +1941,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="105625088"/>
+        <c:crossAx val="166275712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1941,7 +1949,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105625088"/>
+        <c:axId val="166275712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1963,7 +1971,15 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" sz="1400" baseline="0"/>
-                  <a:t> Rate of Reaction (ml)</a:t>
+                  <a:t> Rate of Reaction (ml s</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1400" baseline="30000"/>
+                  <a:t>-1</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1400" baseline="0"/>
+                  <a:t>)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1985,7 +2001,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="105622912"/>
+        <c:crossAx val="166273792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2178,11 +2194,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="100522240"/>
-        <c:axId val="100528512"/>
+        <c:axId val="102395264"/>
+        <c:axId val="102397440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="100522240"/>
+        <c:axId val="102395264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2222,7 +2238,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="100528512"/>
+        <c:crossAx val="102397440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2230,7 +2246,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100528512"/>
+        <c:axId val="102397440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2271,7 +2287,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="100522240"/>
+        <c:crossAx val="102395264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2625,11 +2641,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="100952704"/>
-        <c:axId val="100971264"/>
+        <c:axId val="108003328"/>
+        <c:axId val="108005248"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="100952704"/>
+        <c:axId val="108003328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2657,7 +2673,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100971264"/>
+        <c:crossAx val="108005248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2665,7 +2681,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100971264"/>
+        <c:axId val="108005248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2694,7 +2710,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100952704"/>
+        <c:crossAx val="108003328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2881,11 +2897,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="100992896"/>
-        <c:axId val="100999168"/>
+        <c:axId val="108022784"/>
+        <c:axId val="108041344"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="100992896"/>
+        <c:axId val="108022784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2925,7 +2941,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="100999168"/>
+        <c:crossAx val="108041344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2933,7 +2949,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100999168"/>
+        <c:axId val="108041344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2974,7 +2990,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="100992896"/>
+        <c:crossAx val="108022784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3328,11 +3344,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="101046912"/>
-        <c:axId val="105382656"/>
+        <c:axId val="108088704"/>
+        <c:axId val="108094976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101046912"/>
+        <c:axId val="108088704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3360,7 +3376,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105382656"/>
+        <c:crossAx val="108094976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3368,7 +3384,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105382656"/>
+        <c:axId val="108094976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3397,7 +3413,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101046912"/>
+        <c:crossAx val="108088704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3581,11 +3597,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="105416192"/>
-        <c:axId val="105418112"/>
+        <c:axId val="108124800"/>
+        <c:axId val="108331776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="105416192"/>
+        <c:axId val="108124800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3625,7 +3641,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="105418112"/>
+        <c:crossAx val="108331776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3633,7 +3649,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105418112"/>
+        <c:axId val="108331776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -3674,7 +3690,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="105416192"/>
+        <c:crossAx val="108124800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3734,6 +3750,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4028,11 +4045,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="98616832"/>
-        <c:axId val="98618752"/>
+        <c:axId val="143161984"/>
+        <c:axId val="143164160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="98616832"/>
+        <c:axId val="143161984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4054,13 +4071,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98618752"/>
+        <c:crossAx val="143164160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4068,7 +4086,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98618752"/>
+        <c:axId val="143164160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4091,19 +4109,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98616832"/>
+        <c:crossAx val="143161984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4161,6 +4181,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4285,11 +4306,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="98677504"/>
-        <c:axId val="98679424"/>
+        <c:axId val="149231488"/>
+        <c:axId val="149233664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="98677504"/>
+        <c:axId val="149231488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4313,6 +4334,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -4329,7 +4351,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98679424"/>
+        <c:crossAx val="149233664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4337,7 +4359,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98679424"/>
+        <c:axId val="149233664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -4361,6 +4383,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -4377,7 +4400,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98677504"/>
+        <c:crossAx val="149231488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4437,6 +4460,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4731,11 +4755,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="98772480"/>
-        <c:axId val="98774400"/>
+        <c:axId val="149559936"/>
+        <c:axId val="149562112"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="98772480"/>
+        <c:axId val="149559936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4757,13 +4781,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98774400"/>
+        <c:crossAx val="149562112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4771,7 +4796,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98774400"/>
+        <c:axId val="149562112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4794,19 +4819,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98772480"/>
+        <c:crossAx val="149559936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5399,15 +5426,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
+      <xdr:colOff>481263</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>4</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>113109</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>145382</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -5416,8 +5443,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="5153025" y="3952875"/>
-          <a:ext cx="4829175" cy="2771779"/>
+          <a:off x="5142560" y="3958828"/>
+          <a:ext cx="5430190" cy="2717132"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -7604,10 +7631,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M24"/>
+  <dimension ref="B2:M32"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F15"/>
+    <sheetView topLeftCell="E16" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8098,6 +8125,20 @@
       <c r="F24">
         <f>100/227.14</f>
         <v>0.44025711015232899</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <f>98/255</f>
+        <v>0.3843137254901961</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <v>98</v>
+      </c>
+      <c r="E32">
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -9116,8 +9157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="E4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9164,7 +9205,7 @@
         <v>3.2</v>
       </c>
       <c r="D7" s="17">
-        <v>0.44025700000000001</v>
+        <v>0.38431399999999999</v>
       </c>
     </row>
     <row r="8" spans="3:4" x14ac:dyDescent="0.25">

</xml_diff>